<commit_message>
A1#111ELIOSSUITEXX: Correzione Checklist e test case 31,39,47
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111ELIOSSUITEXX/eliossuite/0012023/3/report-checklist.xlsx
+++ b/GATEWAY/A1#111ELIOSSUITEXX/eliossuite/0012023/3/report-checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\FSE2\TEST\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\fse_git\it-fse-accreditamento\GATEWAY\A1#111ELIOSSUITEXX\eliossuite\0012023\3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C822377-E600-4682-902A-118CD7B35B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E7D2FE4-F99B-4514-885E-3ECE79BB55B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1347" uniqueCount="567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1373" uniqueCount="576">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -2901,6 +2901,33 @@
   <si>
     <t>2.16.840.1.113883.2.9.2.190.4.4.7e65708e07d54dd2321731ec5710c9b15c0dd852734415d149e630696dbf64a5.1e943af217^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
+  <si>
+    <t>2023-07-04T17:16:51:00Z</t>
+  </si>
+  <si>
+    <t>8f8e796d00250a1d</t>
+  </si>
+  <si>
+    <t>UNKNOWN_WORKFLOW_ID</t>
+  </si>
+  <si>
+    <t>2023-07-04T17:24:05:00Z</t>
+  </si>
+  <si>
+    <t>1c3e4c1fb46d7a33</t>
+  </si>
+  <si>
+    <t>Errore JWT</t>
+  </si>
+  <si>
+    <t>Errore Timeout</t>
+  </si>
+  <si>
+    <t>Viene mostrato un messaggio di errore all'operatore invitandolo a riprovare le operazioni</t>
+  </si>
+  <si>
+    <t>Il sistema attende un numero di millisecondi configurabile (default 30000) Dopo tale tempo viene mostrato un messaggio di errore all'operatore invitandolo a riprovare</t>
+  </si>
 </sst>
 </file>
 
@@ -2909,11 +2936,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3236,138 +3270,144 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale 2" xfId="1" xr:uid="{623A807D-3875-4C37-9C2C-4B1DEE1F1503}"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -5828,7 +5868,7 @@
       <pane xSplit="1" ySplit="9" topLeftCell="M10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
+      <selection pane="bottomRight" activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -6294,17 +6334,37 @@
       <c r="E15" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="F15" s="23"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="25"/>
+      <c r="F15" s="50" t="s">
+        <v>567</v>
+      </c>
+      <c r="G15" s="50" t="s">
+        <v>567</v>
+      </c>
+      <c r="H15" s="51" t="s">
+        <v>568</v>
+      </c>
+      <c r="I15" s="51" t="s">
+        <v>569</v>
+      </c>
+      <c r="J15" s="25" t="s">
+        <v>73</v>
+      </c>
       <c r="K15" s="25"/>
-      <c r="L15" s="25"/>
-      <c r="M15" s="25"/>
-      <c r="N15" s="25"/>
-      <c r="O15" s="25"/>
-      <c r="P15" s="25"/>
+      <c r="L15" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="M15" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="N15" s="25" t="s">
+        <v>572</v>
+      </c>
+      <c r="O15" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="P15" s="25" t="s">
+        <v>574</v>
+      </c>
       <c r="Q15" s="25"/>
       <c r="R15" s="26"/>
       <c r="S15" s="27"/>
@@ -6328,17 +6388,37 @@
       <c r="E16" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="F16" s="23"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="25"/>
+      <c r="F16" s="50" t="s">
+        <v>570</v>
+      </c>
+      <c r="G16" s="50" t="s">
+        <v>570</v>
+      </c>
+      <c r="H16" s="51" t="s">
+        <v>571</v>
+      </c>
+      <c r="I16" s="51" t="s">
+        <v>569</v>
+      </c>
+      <c r="J16" s="25" t="s">
+        <v>73</v>
+      </c>
       <c r="K16" s="25"/>
-      <c r="L16" s="25"/>
-      <c r="M16" s="25"/>
-      <c r="N16" s="25"/>
-      <c r="O16" s="25"/>
-      <c r="P16" s="25"/>
+      <c r="L16" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="M16" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="N16" s="25" t="s">
+        <v>572</v>
+      </c>
+      <c r="O16" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="P16" s="25" t="s">
+        <v>574</v>
+      </c>
       <c r="Q16" s="25"/>
       <c r="R16" s="26"/>
       <c r="S16" s="27"/>
@@ -6366,13 +6446,25 @@
       <c r="G17" s="24"/>
       <c r="H17" s="24"/>
       <c r="I17" s="24"/>
-      <c r="J17" s="25"/>
+      <c r="J17" s="25" t="s">
+        <v>73</v>
+      </c>
       <c r="K17" s="25"/>
-      <c r="L17" s="25"/>
-      <c r="M17" s="25"/>
-      <c r="N17" s="25"/>
-      <c r="O17" s="25"/>
-      <c r="P17" s="25"/>
+      <c r="L17" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="M17" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="N17" s="25" t="s">
+        <v>573</v>
+      </c>
+      <c r="O17" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="P17" s="25" t="s">
+        <v>575</v>
+      </c>
       <c r="Q17" s="25"/>
       <c r="R17" s="26" t="s">
         <v>73</v>

</xml_diff>

<commit_message>
A1#111ELIOSSUITEXX: Campi mancanti su checklist
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111ELIOSSUITEXX/eliossuite/0012023/3/report-checklist.xlsx
+++ b/GATEWAY/A1#111ELIOSSUITEXX/eliossuite/0012023/3/report-checklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\FSE2\TEST\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\fse_git\it-fse-accreditamento\GATEWAY\A1#111ELIOSSUITEXX\eliossuite\0012023\3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69296197-5E2E-4CB4-A952-E2D3CC465200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B815D58E-1F72-4A80-B6B2-E1D1BCB4A049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1666" uniqueCount="685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1686" uniqueCount="688">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -3402,6 +3402,15 @@
   </si>
   <si>
     <t>Elios Suite SRL</t>
+  </si>
+  <si>
+    <t>L'utente viene invitato a rigenerare il token attenzionando i parametri inseriti</t>
+  </si>
+  <si>
+    <t>L'utente viene invitato a riprovare dopo errore di timeout</t>
+  </si>
+  <si>
+    <t>L'utente viene inviato a compilare tutti i campi necessari per la validazione del cda2</t>
   </si>
 </sst>
 </file>
@@ -3870,28 +3879,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3918,6 +3905,28 @@
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
@@ -6380,10 +6389,10 @@
   <dimension ref="A1:T830"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B223" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="C21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomRight" activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -6422,14 +6431,14 @@
       <c r="T1" s="15"/>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="42" t="s">
+      <c r="B2" s="50"/>
+      <c r="C2" s="51" t="s">
         <v>684</v>
       </c>
-      <c r="D2" s="41"/>
+      <c r="D2" s="50"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -6447,11 +6456,11 @@
       <c r="T2" s="15"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="49" t="s">
+      <c r="B3" s="53"/>
+      <c r="C3" s="58" t="s">
         <v>681</v>
       </c>
       <c r="D3" s="59"/>
@@ -6472,9 +6481,9 @@
       <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A4" s="45"/>
-      <c r="B4" s="46"/>
-      <c r="C4" s="49" t="s">
+      <c r="A4" s="54"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="58" t="s">
         <v>682</v>
       </c>
       <c r="D4" s="59"/>
@@ -6496,9 +6505,9 @@
       <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A5" s="47"/>
-      <c r="B5" s="48"/>
-      <c r="C5" s="49" t="s">
+      <c r="A5" s="56"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="58" t="s">
         <v>683</v>
       </c>
       <c r="D5" s="59"/>
@@ -6519,8 +6528,8 @@
       <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A6" s="38"/>
-      <c r="B6" s="39"/>
+      <c r="A6" s="47"/>
+      <c r="B6" s="48"/>
       <c r="C6" s="16"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -6867,11 +6876,21 @@
         <v>70</v>
       </c>
       <c r="K15" s="25"/>
-      <c r="L15" s="25"/>
-      <c r="M15" s="25"/>
-      <c r="N15" s="25"/>
-      <c r="O15" s="25"/>
-      <c r="P15" s="25"/>
+      <c r="L15" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="M15" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="N15" s="25" t="s">
+        <v>573</v>
+      </c>
+      <c r="O15" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="P15" s="25" t="s">
+        <v>685</v>
+      </c>
       <c r="Q15" s="25"/>
       <c r="R15" s="26"/>
       <c r="S15" s="27"/>
@@ -6911,11 +6930,21 @@
         <v>70</v>
       </c>
       <c r="K16" s="25"/>
-      <c r="L16" s="25"/>
-      <c r="M16" s="25"/>
-      <c r="N16" s="25"/>
-      <c r="O16" s="25"/>
-      <c r="P16" s="25"/>
+      <c r="L16" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="M16" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="N16" s="25" t="s">
+        <v>573</v>
+      </c>
+      <c r="O16" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="P16" s="25" t="s">
+        <v>685</v>
+      </c>
       <c r="Q16" s="25"/>
       <c r="R16" s="26"/>
       <c r="S16" s="27"/>
@@ -6947,11 +6976,21 @@
         <v>70</v>
       </c>
       <c r="K17" s="25"/>
-      <c r="L17" s="25"/>
-      <c r="M17" s="25"/>
-      <c r="N17" s="25"/>
-      <c r="O17" s="25"/>
-      <c r="P17" s="25"/>
+      <c r="L17" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="M17" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="N17" s="25" t="s">
+        <v>580</v>
+      </c>
+      <c r="O17" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="P17" s="25" t="s">
+        <v>686</v>
+      </c>
       <c r="Q17" s="25"/>
       <c r="R17" s="26" t="s">
         <v>70</v>
@@ -13856,19 +13895,19 @@
       </c>
     </row>
     <row r="214" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A214" s="50">
+      <c r="A214" s="38">
         <v>32</v>
       </c>
-      <c r="B214" s="51" t="s">
+      <c r="B214" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="C214" s="51" t="s">
+      <c r="C214" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="D214" s="51" t="s">
+      <c r="D214" s="39" t="s">
         <v>569</v>
       </c>
-      <c r="E214" s="52" t="s">
+      <c r="E214" s="40" t="s">
         <v>570</v>
       </c>
       <c r="F214" s="33" t="s">
@@ -13886,7 +13925,7 @@
       <c r="J214" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="K214" s="53"/>
+      <c r="K214" s="41"/>
       <c r="L214" s="25" t="s">
         <v>70</v>
       </c>
@@ -13902,27 +13941,27 @@
       <c r="P214" s="25" t="s">
         <v>574</v>
       </c>
-      <c r="Q214" s="53"/>
-      <c r="R214" s="54"/>
-      <c r="S214" s="55"/>
-      <c r="T214" s="56" t="s">
+      <c r="Q214" s="41"/>
+      <c r="R214" s="42"/>
+      <c r="S214" s="43"/>
+      <c r="T214" s="44" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="215" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A215" s="50">
+      <c r="A215" s="38">
         <v>40</v>
       </c>
-      <c r="B215" s="51" t="s">
+      <c r="B215" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="C215" s="51" t="s">
+      <c r="C215" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="D215" s="51" t="s">
+      <c r="D215" s="39" t="s">
         <v>575</v>
       </c>
-      <c r="E215" s="52" t="s">
+      <c r="E215" s="40" t="s">
         <v>576</v>
       </c>
       <c r="F215" s="33" t="s">
@@ -13940,7 +13979,7 @@
       <c r="J215" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="K215" s="53"/>
+      <c r="K215" s="41"/>
       <c r="L215" s="25" t="s">
         <v>70</v>
       </c>
@@ -13956,37 +13995,37 @@
       <c r="P215" s="25" t="s">
         <v>574</v>
       </c>
-      <c r="Q215" s="53"/>
-      <c r="R215" s="54"/>
-      <c r="S215" s="55"/>
-      <c r="T215" s="56" t="s">
+      <c r="Q215" s="41"/>
+      <c r="R215" s="42"/>
+      <c r="S215" s="43"/>
+      <c r="T215" s="44" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="216" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A216" s="50">
+      <c r="A216" s="38">
         <v>48</v>
       </c>
-      <c r="B216" s="51" t="s">
+      <c r="B216" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="C216" s="51" t="s">
+      <c r="C216" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="D216" s="51" t="s">
+      <c r="D216" s="39" t="s">
         <v>579</v>
       </c>
-      <c r="E216" s="52" t="s">
+      <c r="E216" s="40" t="s">
         <v>69</v>
       </c>
       <c r="F216" s="33"/>
       <c r="G216" s="33"/>
-      <c r="H216" s="57"/>
-      <c r="I216" s="57"/>
+      <c r="H216" s="45"/>
+      <c r="I216" s="45"/>
       <c r="J216" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="K216" s="53"/>
+      <c r="K216" s="41"/>
       <c r="L216" s="25" t="s">
         <v>70</v>
       </c>
@@ -14002,29 +14041,29 @@
       <c r="P216" s="25" t="s">
         <v>581</v>
       </c>
-      <c r="Q216" s="53"/>
-      <c r="R216" s="54" t="s">
+      <c r="Q216" s="41"/>
+      <c r="R216" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="S216" s="55"/>
-      <c r="T216" s="56" t="s">
+      <c r="S216" s="43"/>
+      <c r="T216" s="44" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="217" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A217" s="50">
+      <c r="A217" s="38">
         <v>147</v>
       </c>
-      <c r="B217" s="51" t="s">
+      <c r="B217" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="C217" s="51" t="s">
+      <c r="C217" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="D217" s="51" t="s">
+      <c r="D217" s="39" t="s">
         <v>582</v>
       </c>
-      <c r="E217" s="52" t="s">
+      <c r="E217" s="40" t="s">
         <v>583</v>
       </c>
       <c r="F217" s="33" t="s">
@@ -14042,144 +14081,144 @@
       <c r="J217" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="K217" s="53"/>
-      <c r="L217" s="53"/>
-      <c r="M217" s="53"/>
-      <c r="N217" s="53"/>
-      <c r="O217" s="53"/>
-      <c r="P217" s="53"/>
-      <c r="Q217" s="53"/>
-      <c r="R217" s="54"/>
-      <c r="S217" s="55"/>
-      <c r="T217" s="56" t="s">
+      <c r="K217" s="41"/>
+      <c r="L217" s="41"/>
+      <c r="M217" s="41"/>
+      <c r="N217" s="41"/>
+      <c r="O217" s="41"/>
+      <c r="P217" s="41"/>
+      <c r="Q217" s="41"/>
+      <c r="R217" s="42"/>
+      <c r="S217" s="43"/>
+      <c r="T217" s="44" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="218" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A218" s="50">
+      <c r="A218" s="38">
         <v>148</v>
       </c>
-      <c r="B218" s="51" t="s">
+      <c r="B218" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="C218" s="51" t="s">
+      <c r="C218" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="D218" s="51" t="s">
+      <c r="D218" s="39" t="s">
         <v>587</v>
       </c>
-      <c r="E218" s="52" t="s">
+      <c r="E218" s="40" t="s">
         <v>588</v>
       </c>
-      <c r="F218" s="58"/>
-      <c r="G218" s="57"/>
-      <c r="H218" s="57"/>
-      <c r="I218" s="57"/>
+      <c r="F218" s="46"/>
+      <c r="G218" s="45"/>
+      <c r="H218" s="45"/>
+      <c r="I218" s="45"/>
       <c r="J218" s="25" t="s">
         <v>515</v>
       </c>
       <c r="K218" s="37" t="s">
         <v>521</v>
       </c>
-      <c r="L218" s="53"/>
-      <c r="M218" s="53"/>
-      <c r="N218" s="53"/>
-      <c r="O218" s="53"/>
-      <c r="P218" s="53"/>
-      <c r="Q218" s="53"/>
-      <c r="R218" s="54"/>
-      <c r="S218" s="55"/>
-      <c r="T218" s="56" t="s">
+      <c r="L218" s="41"/>
+      <c r="M218" s="41"/>
+      <c r="N218" s="41"/>
+      <c r="O218" s="41"/>
+      <c r="P218" s="41"/>
+      <c r="Q218" s="41"/>
+      <c r="R218" s="42"/>
+      <c r="S218" s="43"/>
+      <c r="T218" s="44" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="219" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A219" s="50">
+      <c r="A219" s="38">
         <v>149</v>
       </c>
-      <c r="B219" s="51" t="s">
+      <c r="B219" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="C219" s="51" t="s">
+      <c r="C219" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="D219" s="51" t="s">
+      <c r="D219" s="39" t="s">
         <v>589</v>
       </c>
-      <c r="E219" s="52" t="s">
+      <c r="E219" s="40" t="s">
         <v>590</v>
       </c>
-      <c r="F219" s="58"/>
-      <c r="G219" s="57"/>
-      <c r="H219" s="57"/>
-      <c r="I219" s="57"/>
+      <c r="F219" s="46"/>
+      <c r="G219" s="45"/>
+      <c r="H219" s="45"/>
+      <c r="I219" s="45"/>
       <c r="J219" s="25" t="s">
         <v>515</v>
       </c>
       <c r="K219" s="37" t="s">
         <v>521</v>
       </c>
-      <c r="L219" s="53"/>
-      <c r="M219" s="53"/>
-      <c r="N219" s="53"/>
-      <c r="O219" s="53"/>
-      <c r="P219" s="53"/>
-      <c r="Q219" s="53"/>
-      <c r="R219" s="54"/>
-      <c r="S219" s="55"/>
-      <c r="T219" s="56" t="s">
+      <c r="L219" s="41"/>
+      <c r="M219" s="41"/>
+      <c r="N219" s="41"/>
+      <c r="O219" s="41"/>
+      <c r="P219" s="41"/>
+      <c r="Q219" s="41"/>
+      <c r="R219" s="42"/>
+      <c r="S219" s="43"/>
+      <c r="T219" s="44" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="220" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A220" s="50">
+      <c r="A220" s="38">
         <v>150</v>
       </c>
-      <c r="B220" s="51" t="s">
+      <c r="B220" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="C220" s="51" t="s">
+      <c r="C220" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="D220" s="51" t="s">
+      <c r="D220" s="39" t="s">
         <v>591</v>
       </c>
-      <c r="E220" s="52" t="s">
+      <c r="E220" s="40" t="s">
         <v>592</v>
       </c>
-      <c r="F220" s="58"/>
-      <c r="G220" s="57"/>
-      <c r="H220" s="57"/>
-      <c r="I220" s="57"/>
+      <c r="F220" s="46"/>
+      <c r="G220" s="45"/>
+      <c r="H220" s="45"/>
+      <c r="I220" s="45"/>
       <c r="J220" s="25" t="s">
         <v>515</v>
       </c>
       <c r="K220" s="37" t="s">
         <v>521</v>
       </c>
-      <c r="L220" s="53"/>
-      <c r="M220" s="53"/>
-      <c r="N220" s="53"/>
-      <c r="O220" s="53"/>
-      <c r="P220" s="53"/>
-      <c r="Q220" s="53"/>
-      <c r="R220" s="54"/>
-      <c r="S220" s="55"/>
-      <c r="T220" s="56" t="s">
+      <c r="L220" s="41"/>
+      <c r="M220" s="41"/>
+      <c r="N220" s="41"/>
+      <c r="O220" s="41"/>
+      <c r="P220" s="41"/>
+      <c r="Q220" s="41"/>
+      <c r="R220" s="42"/>
+      <c r="S220" s="43"/>
+      <c r="T220" s="44" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="221" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A221" s="50">
+      <c r="A221" s="38">
         <v>151</v>
       </c>
-      <c r="B221" s="51" t="s">
+      <c r="B221" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="C221" s="51" t="s">
+      <c r="C221" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="D221" s="51" t="s">
+      <c r="D221" s="39" t="s">
         <v>593</v>
       </c>
       <c r="E221" s="22" t="s">
@@ -14200,8 +14239,8 @@
       <c r="J221" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="K221" s="53"/>
-      <c r="L221" s="53" t="s">
+      <c r="K221" s="41"/>
+      <c r="L221" s="41" t="s">
         <v>70</v>
       </c>
       <c r="M221" s="25" t="s">
@@ -14216,27 +14255,27 @@
       <c r="P221" s="25" t="s">
         <v>519</v>
       </c>
-      <c r="Q221" s="53"/>
-      <c r="R221" s="54"/>
-      <c r="S221" s="55"/>
-      <c r="T221" s="56" t="s">
+      <c r="Q221" s="41"/>
+      <c r="R221" s="42"/>
+      <c r="S221" s="43"/>
+      <c r="T221" s="44" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="222" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A222" s="50">
+      <c r="A222" s="38">
         <v>152</v>
       </c>
-      <c r="B222" s="51" t="s">
+      <c r="B222" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="C222" s="51" t="s">
+      <c r="C222" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="D222" s="51" t="s">
+      <c r="D222" s="39" t="s">
         <v>598</v>
       </c>
-      <c r="E222" s="52" t="s">
+      <c r="E222" s="40" t="s">
         <v>599</v>
       </c>
       <c r="F222" s="33" t="s">
@@ -14254,7 +14293,7 @@
       <c r="J222" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="K222" s="53"/>
+      <c r="K222" s="41"/>
       <c r="L222" s="25" t="s">
         <v>70</v>
       </c>
@@ -14270,27 +14309,27 @@
       <c r="P222" s="25" t="s">
         <v>603</v>
       </c>
-      <c r="Q222" s="53"/>
-      <c r="R222" s="54"/>
-      <c r="S222" s="55"/>
-      <c r="T222" s="56" t="s">
+      <c r="Q222" s="41"/>
+      <c r="R222" s="42"/>
+      <c r="S222" s="43"/>
+      <c r="T222" s="44" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="223" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A223" s="50">
+      <c r="A223" s="38">
         <v>153</v>
       </c>
-      <c r="B223" s="51" t="s">
+      <c r="B223" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="C223" s="51" t="s">
+      <c r="C223" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="D223" s="51" t="s">
+      <c r="D223" s="39" t="s">
         <v>604</v>
       </c>
-      <c r="E223" s="52" t="s">
+      <c r="E223" s="40" t="s">
         <v>605</v>
       </c>
       <c r="F223" s="33" t="s">
@@ -14308,7 +14347,7 @@
       <c r="J223" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="K223" s="53"/>
+      <c r="K223" s="41"/>
       <c r="L223" s="25" t="s">
         <v>70</v>
       </c>
@@ -14324,27 +14363,27 @@
       <c r="P223" s="25" t="s">
         <v>519</v>
       </c>
-      <c r="Q223" s="53"/>
-      <c r="R223" s="54"/>
-      <c r="S223" s="55"/>
-      <c r="T223" s="56" t="s">
+      <c r="Q223" s="41"/>
+      <c r="R223" s="42"/>
+      <c r="S223" s="43"/>
+      <c r="T223" s="44" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="224" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A224" s="50">
+      <c r="A224" s="38">
         <v>154</v>
       </c>
-      <c r="B224" s="51" t="s">
+      <c r="B224" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="C224" s="51" t="s">
+      <c r="C224" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="D224" s="51" t="s">
+      <c r="D224" s="39" t="s">
         <v>609</v>
       </c>
-      <c r="E224" s="52" t="s">
+      <c r="E224" s="40" t="s">
         <v>610</v>
       </c>
       <c r="F224" s="33" t="s">
@@ -14362,7 +14401,7 @@
       <c r="J224" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="K224" s="53"/>
+      <c r="K224" s="41"/>
       <c r="L224" s="25" t="s">
         <v>70</v>
       </c>
@@ -14378,27 +14417,27 @@
       <c r="P224" s="25" t="s">
         <v>519</v>
       </c>
-      <c r="Q224" s="53"/>
-      <c r="R224" s="54"/>
-      <c r="S224" s="55"/>
-      <c r="T224" s="56" t="s">
+      <c r="Q224" s="41"/>
+      <c r="R224" s="42"/>
+      <c r="S224" s="43"/>
+      <c r="T224" s="44" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="225" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A225" s="50">
+      <c r="A225" s="38">
         <v>155</v>
       </c>
-      <c r="B225" s="51" t="s">
+      <c r="B225" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="C225" s="51" t="s">
+      <c r="C225" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="D225" s="51" t="s">
+      <c r="D225" s="39" t="s">
         <v>614</v>
       </c>
-      <c r="E225" s="52" t="s">
+      <c r="E225" s="40" t="s">
         <v>615</v>
       </c>
       <c r="F225" s="33" t="s">
@@ -14416,7 +14455,7 @@
       <c r="J225" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="K225" s="53"/>
+      <c r="K225" s="41"/>
       <c r="L225" s="25" t="s">
         <v>70</v>
       </c>
@@ -14432,27 +14471,27 @@
       <c r="P225" s="25" t="s">
         <v>519</v>
       </c>
-      <c r="Q225" s="53"/>
-      <c r="R225" s="54"/>
-      <c r="S225" s="55"/>
-      <c r="T225" s="56" t="s">
+      <c r="Q225" s="41"/>
+      <c r="R225" s="42"/>
+      <c r="S225" s="43"/>
+      <c r="T225" s="44" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="226" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A226" s="50">
+      <c r="A226" s="38">
         <v>156</v>
       </c>
-      <c r="B226" s="51" t="s">
+      <c r="B226" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="C226" s="51" t="s">
+      <c r="C226" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="D226" s="51" t="s">
+      <c r="D226" s="39" t="s">
         <v>619</v>
       </c>
-      <c r="E226" s="52" t="s">
+      <c r="E226" s="40" t="s">
         <v>620</v>
       </c>
       <c r="F226" s="33" t="s">
@@ -14470,7 +14509,7 @@
       <c r="J226" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="K226" s="53"/>
+      <c r="K226" s="41"/>
       <c r="L226" s="25" t="s">
         <v>70</v>
       </c>
@@ -14486,65 +14525,65 @@
       <c r="P226" s="25" t="s">
         <v>519</v>
       </c>
-      <c r="Q226" s="53"/>
-      <c r="R226" s="54"/>
-      <c r="S226" s="55"/>
-      <c r="T226" s="56" t="s">
+      <c r="Q226" s="41"/>
+      <c r="R226" s="42"/>
+      <c r="S226" s="43"/>
+      <c r="T226" s="44" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="227" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A227" s="50">
+      <c r="A227" s="38">
         <v>157</v>
       </c>
-      <c r="B227" s="51" t="s">
+      <c r="B227" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="C227" s="51" t="s">
+      <c r="C227" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="D227" s="51" t="s">
+      <c r="D227" s="39" t="s">
         <v>625</v>
       </c>
-      <c r="E227" s="52" t="s">
+      <c r="E227" s="40" t="s">
         <v>626</v>
       </c>
-      <c r="F227" s="58"/>
-      <c r="G227" s="57"/>
-      <c r="H227" s="57"/>
-      <c r="I227" s="57"/>
+      <c r="F227" s="46"/>
+      <c r="G227" s="45"/>
+      <c r="H227" s="45"/>
+      <c r="I227" s="45"/>
       <c r="J227" s="25" t="s">
         <v>515</v>
       </c>
       <c r="K227" s="25" t="s">
         <v>627</v>
       </c>
-      <c r="L227" s="53"/>
-      <c r="M227" s="53"/>
-      <c r="N227" s="53"/>
-      <c r="O227" s="53"/>
-      <c r="P227" s="53"/>
-      <c r="Q227" s="53"/>
-      <c r="R227" s="54"/>
-      <c r="S227" s="55"/>
-      <c r="T227" s="56" t="s">
+      <c r="L227" s="41"/>
+      <c r="M227" s="41"/>
+      <c r="N227" s="41"/>
+      <c r="O227" s="41"/>
+      <c r="P227" s="41"/>
+      <c r="Q227" s="41"/>
+      <c r="R227" s="42"/>
+      <c r="S227" s="43"/>
+      <c r="T227" s="44" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="228" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A228" s="50">
+      <c r="A228" s="38">
         <v>158</v>
       </c>
-      <c r="B228" s="51" t="s">
+      <c r="B228" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="C228" s="51" t="s">
+      <c r="C228" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="D228" s="51" t="s">
+      <c r="D228" s="39" t="s">
         <v>628</v>
       </c>
-      <c r="E228" s="52" t="s">
+      <c r="E228" s="40" t="s">
         <v>629</v>
       </c>
       <c r="F228" s="33" t="s">
@@ -14562,7 +14601,7 @@
       <c r="J228" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="K228" s="53"/>
+      <c r="K228" s="41"/>
       <c r="L228" s="25" t="s">
         <v>70</v>
       </c>
@@ -14578,27 +14617,27 @@
       <c r="P228" s="25" t="s">
         <v>633</v>
       </c>
-      <c r="Q228" s="53"/>
-      <c r="R228" s="54"/>
-      <c r="S228" s="55"/>
-      <c r="T228" s="56" t="s">
+      <c r="Q228" s="41"/>
+      <c r="R228" s="42"/>
+      <c r="S228" s="43"/>
+      <c r="T228" s="44" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="229" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A229" s="50">
+      <c r="A229" s="38">
         <v>159</v>
       </c>
-      <c r="B229" s="51" t="s">
+      <c r="B229" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="C229" s="51" t="s">
+      <c r="C229" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="D229" s="51" t="s">
+      <c r="D229" s="39" t="s">
         <v>634</v>
       </c>
-      <c r="E229" s="52" t="s">
+      <c r="E229" s="40" t="s">
         <v>635</v>
       </c>
       <c r="F229" s="33" t="s">
@@ -14616,7 +14655,7 @@
       <c r="J229" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="K229" s="53"/>
+      <c r="K229" s="41"/>
       <c r="L229" s="25" t="s">
         <v>70</v>
       </c>
@@ -14632,27 +14671,27 @@
       <c r="P229" s="25" t="s">
         <v>633</v>
       </c>
-      <c r="Q229" s="53"/>
-      <c r="R229" s="54"/>
-      <c r="S229" s="55"/>
-      <c r="T229" s="56" t="s">
+      <c r="Q229" s="41"/>
+      <c r="R229" s="42"/>
+      <c r="S229" s="43"/>
+      <c r="T229" s="44" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="230" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A230" s="50">
+      <c r="A230" s="38">
         <v>160</v>
       </c>
-      <c r="B230" s="51" t="s">
+      <c r="B230" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="C230" s="51" t="s">
+      <c r="C230" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="D230" s="51" t="s">
+      <c r="D230" s="39" t="s">
         <v>639</v>
       </c>
-      <c r="E230" s="52" t="s">
+      <c r="E230" s="40" t="s">
         <v>640</v>
       </c>
       <c r="F230" s="33" t="s">
@@ -14670,7 +14709,7 @@
       <c r="J230" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="K230" s="53"/>
+      <c r="K230" s="41"/>
       <c r="L230" s="25" t="s">
         <v>70</v>
       </c>
@@ -14686,27 +14725,27 @@
       <c r="P230" s="25" t="s">
         <v>644</v>
       </c>
-      <c r="Q230" s="53"/>
-      <c r="R230" s="54"/>
-      <c r="S230" s="55"/>
-      <c r="T230" s="56" t="s">
+      <c r="Q230" s="41"/>
+      <c r="R230" s="42"/>
+      <c r="S230" s="43"/>
+      <c r="T230" s="44" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="231" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A231" s="50">
+      <c r="A231" s="38">
         <v>161</v>
       </c>
-      <c r="B231" s="51" t="s">
+      <c r="B231" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="C231" s="51" t="s">
+      <c r="C231" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="D231" s="51" t="s">
+      <c r="D231" s="39" t="s">
         <v>645</v>
       </c>
-      <c r="E231" s="52" t="s">
+      <c r="E231" s="40" t="s">
         <v>646</v>
       </c>
       <c r="F231" s="33" t="s">
@@ -14724,7 +14763,7 @@
       <c r="J231" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="K231" s="53"/>
+      <c r="K231" s="41"/>
       <c r="L231" s="25" t="s">
         <v>70</v>
       </c>
@@ -14740,65 +14779,65 @@
       <c r="P231" s="25" t="s">
         <v>650</v>
       </c>
-      <c r="Q231" s="53"/>
-      <c r="R231" s="54"/>
-      <c r="S231" s="55"/>
-      <c r="T231" s="56" t="s">
+      <c r="Q231" s="41"/>
+      <c r="R231" s="42"/>
+      <c r="S231" s="43"/>
+      <c r="T231" s="44" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="232" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A232" s="50">
+      <c r="A232" s="38">
         <v>162</v>
       </c>
-      <c r="B232" s="51" t="s">
+      <c r="B232" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="C232" s="51" t="s">
+      <c r="C232" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="D232" s="51" t="s">
+      <c r="D232" s="39" t="s">
         <v>651</v>
       </c>
-      <c r="E232" s="52" t="s">
+      <c r="E232" s="40" t="s">
         <v>652</v>
       </c>
-      <c r="F232" s="58"/>
-      <c r="G232" s="57"/>
-      <c r="H232" s="57"/>
-      <c r="I232" s="57"/>
+      <c r="F232" s="46"/>
+      <c r="G232" s="45"/>
+      <c r="H232" s="45"/>
+      <c r="I232" s="45"/>
       <c r="J232" s="25" t="s">
         <v>515</v>
       </c>
       <c r="K232" s="25" t="s">
         <v>653</v>
       </c>
-      <c r="L232" s="53"/>
-      <c r="M232" s="53"/>
-      <c r="N232" s="53"/>
-      <c r="O232" s="53"/>
-      <c r="P232" s="53"/>
-      <c r="Q232" s="53"/>
-      <c r="R232" s="54"/>
-      <c r="S232" s="55"/>
-      <c r="T232" s="56" t="s">
+      <c r="L232" s="41"/>
+      <c r="M232" s="41"/>
+      <c r="N232" s="41"/>
+      <c r="O232" s="41"/>
+      <c r="P232" s="41"/>
+      <c r="Q232" s="41"/>
+      <c r="R232" s="42"/>
+      <c r="S232" s="43"/>
+      <c r="T232" s="44" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="233" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A233" s="50">
+      <c r="A233" s="38">
         <v>163</v>
       </c>
-      <c r="B233" s="51" t="s">
+      <c r="B233" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="C233" s="51" t="s">
+      <c r="C233" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="D233" s="51" t="s">
+      <c r="D233" s="39" t="s">
         <v>654</v>
       </c>
-      <c r="E233" s="52" t="s">
+      <c r="E233" s="40" t="s">
         <v>655</v>
       </c>
       <c r="F233" s="33" t="s">
@@ -14816,38 +14855,48 @@
       <c r="J233" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="K233" s="53"/>
-      <c r="L233" s="53"/>
-      <c r="M233" s="53"/>
-      <c r="N233" s="53"/>
-      <c r="O233" s="53"/>
-      <c r="P233" s="53"/>
-      <c r="Q233" s="53"/>
-      <c r="R233" s="54"/>
-      <c r="S233" s="55"/>
-      <c r="T233" s="56" t="s">
+      <c r="K233" s="41"/>
+      <c r="L233" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="M233" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="N233" s="41" t="s">
+        <v>520</v>
+      </c>
+      <c r="O233" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="P233" s="41" t="s">
+        <v>687</v>
+      </c>
+      <c r="Q233" s="41"/>
+      <c r="R233" s="42"/>
+      <c r="S233" s="43"/>
+      <c r="T233" s="44" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="234" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A234" s="50">
+      <c r="A234" s="38">
         <v>164</v>
       </c>
-      <c r="B234" s="51" t="s">
+      <c r="B234" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="C234" s="51" t="s">
+      <c r="C234" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="D234" s="51" t="s">
+      <c r="D234" s="39" t="s">
         <v>659</v>
       </c>
-      <c r="E234" s="52" t="s">
+      <c r="E234" s="40" t="s">
         <v>660</v>
       </c>
-      <c r="F234" s="58"/>
-      <c r="G234" s="57"/>
-      <c r="H234" s="57"/>
+      <c r="F234" s="46"/>
+      <c r="G234" s="45"/>
+      <c r="H234" s="45"/>
       <c r="I234" s="24"/>
       <c r="J234" s="25" t="s">
         <v>515</v>
@@ -14855,184 +14904,184 @@
       <c r="K234" s="25" t="s">
         <v>661</v>
       </c>
-      <c r="L234" s="53"/>
-      <c r="M234" s="53"/>
-      <c r="N234" s="53"/>
-      <c r="O234" s="53"/>
-      <c r="P234" s="53"/>
-      <c r="Q234" s="53"/>
-      <c r="R234" s="54"/>
-      <c r="S234" s="55"/>
-      <c r="T234" s="56" t="s">
+      <c r="L234" s="41"/>
+      <c r="M234" s="41"/>
+      <c r="N234" s="41"/>
+      <c r="O234" s="41"/>
+      <c r="P234" s="41"/>
+      <c r="Q234" s="41"/>
+      <c r="R234" s="42"/>
+      <c r="S234" s="43"/>
+      <c r="T234" s="44" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="235" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A235" s="50">
+      <c r="A235" s="38">
         <v>165</v>
       </c>
-      <c r="B235" s="51" t="s">
+      <c r="B235" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="C235" s="51" t="s">
+      <c r="C235" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="D235" s="51" t="s">
+      <c r="D235" s="39" t="s">
         <v>662</v>
       </c>
-      <c r="E235" s="52" t="s">
+      <c r="E235" s="40" t="s">
         <v>663</v>
       </c>
-      <c r="F235" s="58"/>
-      <c r="G235" s="57"/>
-      <c r="H235" s="57"/>
-      <c r="I235" s="57"/>
+      <c r="F235" s="46"/>
+      <c r="G235" s="45"/>
+      <c r="H235" s="45"/>
+      <c r="I235" s="45"/>
       <c r="J235" s="25" t="s">
         <v>515</v>
       </c>
       <c r="K235" s="25" t="s">
         <v>664</v>
       </c>
-      <c r="L235" s="53"/>
-      <c r="M235" s="53"/>
-      <c r="N235" s="53"/>
-      <c r="O235" s="53"/>
-      <c r="P235" s="53"/>
-      <c r="Q235" s="53"/>
-      <c r="R235" s="54"/>
-      <c r="S235" s="55"/>
-      <c r="T235" s="56" t="s">
+      <c r="L235" s="41"/>
+      <c r="M235" s="41"/>
+      <c r="N235" s="41"/>
+      <c r="O235" s="41"/>
+      <c r="P235" s="41"/>
+      <c r="Q235" s="41"/>
+      <c r="R235" s="42"/>
+      <c r="S235" s="43"/>
+      <c r="T235" s="44" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="236" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A236" s="50">
+      <c r="A236" s="38">
         <v>166</v>
       </c>
-      <c r="B236" s="51" t="s">
+      <c r="B236" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="C236" s="51" t="s">
+      <c r="C236" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="D236" s="51" t="s">
+      <c r="D236" s="39" t="s">
         <v>665</v>
       </c>
-      <c r="E236" s="52" t="s">
+      <c r="E236" s="40" t="s">
         <v>666</v>
       </c>
-      <c r="F236" s="58"/>
-      <c r="G236" s="57"/>
-      <c r="H236" s="57"/>
-      <c r="I236" s="57"/>
+      <c r="F236" s="46"/>
+      <c r="G236" s="45"/>
+      <c r="H236" s="45"/>
+      <c r="I236" s="45"/>
       <c r="J236" s="25" t="s">
         <v>515</v>
       </c>
       <c r="K236" s="25" t="s">
         <v>664</v>
       </c>
-      <c r="L236" s="53"/>
-      <c r="M236" s="53"/>
-      <c r="N236" s="53"/>
-      <c r="O236" s="53"/>
-      <c r="P236" s="53"/>
-      <c r="Q236" s="53"/>
-      <c r="R236" s="54"/>
-      <c r="S236" s="55"/>
-      <c r="T236" s="56" t="s">
+      <c r="L236" s="41"/>
+      <c r="M236" s="41"/>
+      <c r="N236" s="41"/>
+      <c r="O236" s="41"/>
+      <c r="P236" s="41"/>
+      <c r="Q236" s="41"/>
+      <c r="R236" s="42"/>
+      <c r="S236" s="43"/>
+      <c r="T236" s="44" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="237" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A237" s="50">
+      <c r="A237" s="38">
         <v>167</v>
       </c>
-      <c r="B237" s="51" t="s">
+      <c r="B237" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="C237" s="51" t="s">
+      <c r="C237" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="D237" s="51" t="s">
+      <c r="D237" s="39" t="s">
         <v>667</v>
       </c>
-      <c r="E237" s="52" t="s">
+      <c r="E237" s="40" t="s">
         <v>668</v>
       </c>
-      <c r="F237" s="58"/>
-      <c r="G237" s="57"/>
-      <c r="H237" s="57"/>
-      <c r="I237" s="57"/>
+      <c r="F237" s="46"/>
+      <c r="G237" s="45"/>
+      <c r="H237" s="45"/>
+      <c r="I237" s="45"/>
       <c r="J237" s="25" t="s">
         <v>515</v>
       </c>
       <c r="K237" s="25" t="s">
         <v>661</v>
       </c>
-      <c r="L237" s="53"/>
-      <c r="M237" s="53"/>
-      <c r="N237" s="53"/>
-      <c r="O237" s="53"/>
-      <c r="P237" s="53"/>
-      <c r="Q237" s="53"/>
-      <c r="R237" s="54"/>
-      <c r="S237" s="55"/>
-      <c r="T237" s="56" t="s">
+      <c r="L237" s="41"/>
+      <c r="M237" s="41"/>
+      <c r="N237" s="41"/>
+      <c r="O237" s="41"/>
+      <c r="P237" s="41"/>
+      <c r="Q237" s="41"/>
+      <c r="R237" s="42"/>
+      <c r="S237" s="43"/>
+      <c r="T237" s="44" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="238" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A238" s="50">
+      <c r="A238" s="38">
         <v>168</v>
       </c>
-      <c r="B238" s="51" t="s">
+      <c r="B238" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="C238" s="51" t="s">
+      <c r="C238" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="D238" s="51" t="s">
+      <c r="D238" s="39" t="s">
         <v>669</v>
       </c>
-      <c r="E238" s="52" t="s">
+      <c r="E238" s="40" t="s">
         <v>670</v>
       </c>
-      <c r="F238" s="58"/>
-      <c r="G238" s="57"/>
-      <c r="H238" s="57"/>
-      <c r="I238" s="57"/>
+      <c r="F238" s="46"/>
+      <c r="G238" s="45"/>
+      <c r="H238" s="45"/>
+      <c r="I238" s="45"/>
       <c r="J238" s="25" t="s">
         <v>515</v>
       </c>
       <c r="K238" s="25" t="s">
         <v>661</v>
       </c>
-      <c r="L238" s="53"/>
-      <c r="M238" s="53"/>
-      <c r="N238" s="53"/>
-      <c r="O238" s="53"/>
-      <c r="P238" s="53"/>
-      <c r="Q238" s="53"/>
-      <c r="R238" s="54"/>
-      <c r="S238" s="55"/>
-      <c r="T238" s="56" t="s">
+      <c r="L238" s="41"/>
+      <c r="M238" s="41"/>
+      <c r="N238" s="41"/>
+      <c r="O238" s="41"/>
+      <c r="P238" s="41"/>
+      <c r="Q238" s="41"/>
+      <c r="R238" s="42"/>
+      <c r="S238" s="43"/>
+      <c r="T238" s="44" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="239" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A239" s="50">
+      <c r="A239" s="38">
         <v>169</v>
       </c>
-      <c r="B239" s="51" t="s">
+      <c r="B239" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="C239" s="51" t="s">
+      <c r="C239" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="D239" s="51" t="s">
+      <c r="D239" s="39" t="s">
         <v>671</v>
       </c>
-      <c r="E239" s="52" t="s">
+      <c r="E239" s="40" t="s">
         <v>672</v>
       </c>
       <c r="F239" s="33" t="s">
@@ -15050,7 +15099,7 @@
       <c r="J239" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="K239" s="53"/>
+      <c r="K239" s="41"/>
       <c r="L239" s="25" t="s">
         <v>70</v>
       </c>
@@ -15066,27 +15115,27 @@
       <c r="P239" s="25" t="s">
         <v>650</v>
       </c>
-      <c r="Q239" s="53"/>
-      <c r="R239" s="54"/>
-      <c r="S239" s="55"/>
-      <c r="T239" s="56" t="s">
+      <c r="Q239" s="41"/>
+      <c r="R239" s="42"/>
+      <c r="S239" s="43"/>
+      <c r="T239" s="44" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="240" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A240" s="50">
+      <c r="A240" s="38">
         <v>374</v>
       </c>
-      <c r="B240" s="51" t="s">
+      <c r="B240" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="C240" s="51" t="s">
+      <c r="C240" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="D240" s="51" t="s">
+      <c r="D240" s="39" t="s">
         <v>676</v>
       </c>
-      <c r="E240" s="52" t="s">
+      <c r="E240" s="40" t="s">
         <v>677</v>
       </c>
       <c r="F240" s="33" t="s">
@@ -15101,19 +15150,19 @@
       <c r="I240" s="34" t="s">
         <v>680</v>
       </c>
-      <c r="J240" s="53" t="s">
+      <c r="J240" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="K240" s="53"/>
-      <c r="L240" s="53"/>
-      <c r="M240" s="53"/>
-      <c r="N240" s="53"/>
-      <c r="O240" s="53"/>
-      <c r="P240" s="53"/>
-      <c r="Q240" s="53"/>
-      <c r="R240" s="54"/>
-      <c r="S240" s="55"/>
-      <c r="T240" s="56" t="s">
+      <c r="K240" s="41"/>
+      <c r="L240" s="41"/>
+      <c r="M240" s="41"/>
+      <c r="N240" s="41"/>
+      <c r="O240" s="41"/>
+      <c r="P240" s="41"/>
+      <c r="Q240" s="41"/>
+      <c r="R240" s="42"/>
+      <c r="S240" s="43"/>
+      <c r="T240" s="44" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>

<commit_message>
A1#111ELIOSSUITEXX: Risottomissione check-list con info soluzione
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111ELIOSSUITEXX/eliossuite/0012023/3/report-checklist.xlsx
+++ b/GATEWAY/A1#111ELIOSSUITEXX/eliossuite/0012023/3/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\fse_git\it-fse-accreditamento\GATEWAY\A1#111ELIOSSUITEXX\eliossuite\0012023\3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B815D58E-1F72-4A80-B6B2-E1D1BCB4A049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF5362E6-1970-4952-BDDF-B9739711F555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Sheet1" sheetId="5" state="hidden" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TestCases!$A$9:$T$213</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TestCases!$A$9:$T$240</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1686" uniqueCount="688">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1686" uniqueCount="680">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -2775,17 +2775,11 @@
     <t>Errore di sintassi</t>
   </si>
   <si>
-    <t>CONTROLLO SINTASSI DOCUMENTO</t>
-  </si>
-  <si>
     <t>Errore semantico</t>
   </si>
   <si>
     <t xml:space="preserve">Non vengono gestite le sezioni opzionali.
 </t>
-  </si>
-  <si>
-    <t>CONTROLLO ANAGRAFiCA PAZIENTE</t>
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.190.4.4.7e65708e07d54dd2321731ec5710c9b15c0dd852734415d149e630696dbf64a5.12470852e2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
@@ -2936,6 +2930,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Precondizioni:</t>
     </r>
@@ -2944,6 +2939,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 Il fornitore utilizza un token jwt mancante di campi obbligatori, quindi non valido.
@@ -2956,6 +2952,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Descrizione di Business del caso di test: </t>
     </r>
@@ -2964,6 +2961,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" con un token jwt non valido a causa della mancanza di uno o più campi obbligatori al fine di testare la gestione dell'errore sul token (status code 403), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
@@ -2978,9 +2976,6 @@
   </si>
   <si>
     <t>Errore JWT</t>
-  </si>
-  <si>
-    <t>Viene mostrato un messaggio di errore all'operatore invitandolo a riprovare</t>
   </si>
   <si>
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_RSA_KO</t>
@@ -2993,6 +2988,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Precondizioni:</t>
     </r>
@@ -3001,6 +2997,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 Il fornitore utilizza un token jwt con dei campi valorizzati in maniera errata.
@@ -3013,6 +3010,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Descrizione di Business del caso di test: </t>
     </r>
@@ -3021,6 +3019,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" con un token jwt avente dei campi valorizzati in maniera errata al fine di testare la gestione dell'errore sul token (status code 403), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
@@ -3040,9 +3039,6 @@
     <t>Errore Timeout</t>
   </si>
   <si>
-    <t>Il sistema attende un numero di millisecondi configurabile (default 30000) Dopo tale tempo viene mostrato un messaggio di errore all'operatore</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_RSA_CT1</t>
   </si>
   <si>
@@ -3121,9 +3117,6 @@
     <t>2.16.840.1.113883.2.9.2.190.4.4.f5341f2d8f41dcb8fa4adb36e63b5b1b78960468e091c06cba175e468475c2f1.caca4df247^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>CONTROLLO DATI PAZIENTE</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_RSA_CT7_KO</t>
   </si>
   <si>
@@ -3224,9 +3217,6 @@
     <t>2.16.840.1.113883.2.9.2.190.4.4.f5341f2d8f41dcb8fa4adb36e63b5b1b78960468e091c06cba175e468475c2f1.d4b91e2ecc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>CONTROLLO DATI IMPEGNATIVA</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_RSA_CT13_KO</t>
   </si>
   <si>
@@ -3257,9 +3247,6 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.190.4.4.f5341f2d8f41dcb8fa4adb36e63b5b1b78960468e091c06cba175e468475c2f1.85e09cc537^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>CONTROLLO DATI ACCETTAZIONE</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT15_KO</t>
@@ -3277,9 +3264,6 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.190.4.4.f5341f2d8f41dcb8fa4adb36e63b5b1b78960468e091c06cba175e468475c2f1.15b496ef6c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>CONTROLLO DATI REFERTO</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT16_KO</t>
@@ -3404,13 +3388,13 @@
     <t>Elios Suite SRL</t>
   </si>
   <si>
-    <t>L'utente viene invitato a rigenerare il token attenzionando i parametri inseriti</t>
-  </si>
-  <si>
-    <t>L'utente viene invitato a riprovare dopo errore di timeout</t>
-  </si>
-  <si>
-    <t>L'utente viene inviato a compilare tutti i campi necessari per la validazione del cda2</t>
+    <t>Da backoffice, viene evidenziata una lista di documenti che sono in errore, quindi per ogni documento entrando nel dettaglio, vengono mostrati i parametri necessari alla creazione del token, e con un sistema predittivo si consiglia di correggere quelli formalmente errati. Una volta corretto, il documento viene reinserito nella coda di invio massiva.</t>
+  </si>
+  <si>
+    <t>In automatico il software effettua 3 ulteriori tentativi a distanza di, rispettivamente, 5-10-15 minuti uno dall'altro. Qualora questi non andassero a buon fine, da backoffice, viene evidenziata una lista di documenti che sono in errore, quindi per ogni documento entrando nel dettaglio, vengono mostrate le motivazioni che impediscono l'invio e trattandosi di errore di timeout, l'utente viene invitato a rimettere in coda i documenti affetti da questa problematica.</t>
+  </si>
+  <si>
+    <t>Da backoffice, viene evidenziata una lista di documenti che sono in errore, quindi per ogni documento entrando nel dettaglio, vengono mostrati i parametri errati e con un sistema predittivo si consiglia di correggere quelli formalmente errati. Una volta corretti, il documento viene automaticamente reinserito nella coda di invio massiva.</t>
   </si>
 </sst>
 </file>
@@ -3420,7 +3404,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3501,17 +3485,12 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -3928,7 +3907,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -6389,10 +6368,10 @@
   <dimension ref="A1:T830"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="C21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="J10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="N18" sqref="N18"/>
+      <selection pane="bottomRight" activeCell="P239" sqref="P239"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -6436,7 +6415,7 @@
       </c>
       <c r="B2" s="50"/>
       <c r="C2" s="51" t="s">
-        <v>684</v>
+        <v>676</v>
       </c>
       <c r="D2" s="50"/>
       <c r="F2" s="12"/>
@@ -6461,7 +6440,7 @@
       </c>
       <c r="B3" s="53"/>
       <c r="C3" s="58" t="s">
-        <v>681</v>
+        <v>673</v>
       </c>
       <c r="D3" s="59"/>
       <c r="F3" s="12"/>
@@ -6484,7 +6463,7 @@
       <c r="A4" s="54"/>
       <c r="B4" s="55"/>
       <c r="C4" s="58" t="s">
-        <v>682</v>
+        <v>674</v>
       </c>
       <c r="D4" s="59"/>
       <c r="E4" s="4"/>
@@ -6508,7 +6487,7 @@
       <c r="A5" s="56"/>
       <c r="B5" s="57"/>
       <c r="C5" s="58" t="s">
-        <v>683</v>
+        <v>675</v>
       </c>
       <c r="D5" s="59"/>
       <c r="F5" s="12"/>
@@ -6697,16 +6676,16 @@
         <v>52</v>
       </c>
       <c r="F11" s="33" t="s">
+        <v>527</v>
+      </c>
+      <c r="G11" s="33" t="s">
+        <v>527</v>
+      </c>
+      <c r="H11" s="34" t="s">
+        <v>528</v>
+      </c>
+      <c r="I11" s="34" t="s">
         <v>529</v>
-      </c>
-      <c r="G11" s="33" t="s">
-        <v>529</v>
-      </c>
-      <c r="H11" s="34" t="s">
-        <v>530</v>
-      </c>
-      <c r="I11" s="34" t="s">
-        <v>531</v>
       </c>
       <c r="J11" s="35" t="s">
         <v>517</v>
@@ -6741,16 +6720,16 @@
         <v>54</v>
       </c>
       <c r="F12" s="33" t="s">
+        <v>530</v>
+      </c>
+      <c r="G12" s="33" t="s">
+        <v>530</v>
+      </c>
+      <c r="H12" s="34" t="s">
+        <v>531</v>
+      </c>
+      <c r="I12" s="34" t="s">
         <v>532</v>
-      </c>
-      <c r="G12" s="33" t="s">
-        <v>532</v>
-      </c>
-      <c r="H12" s="34" t="s">
-        <v>533</v>
-      </c>
-      <c r="I12" s="34" t="s">
-        <v>534</v>
       </c>
       <c r="J12" s="35" t="s">
         <v>517</v>
@@ -6792,7 +6771,7 @@
         <v>515</v>
       </c>
       <c r="K13" s="37" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="L13" s="25"/>
       <c r="M13" s="25"/>
@@ -6830,7 +6809,7 @@
         <v>515</v>
       </c>
       <c r="K14" s="36" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="L14" s="25"/>
       <c r="M14" s="25"/>
@@ -6861,16 +6840,16 @@
         <v>65</v>
       </c>
       <c r="F15" s="33" t="s">
+        <v>533</v>
+      </c>
+      <c r="G15" s="33" t="s">
+        <v>533</v>
+      </c>
+      <c r="H15" s="34" t="s">
+        <v>534</v>
+      </c>
+      <c r="I15" s="34" t="s">
         <v>535</v>
-      </c>
-      <c r="G15" s="33" t="s">
-        <v>535</v>
-      </c>
-      <c r="H15" s="34" t="s">
-        <v>536</v>
-      </c>
-      <c r="I15" s="34" t="s">
-        <v>537</v>
       </c>
       <c r="J15" s="25" t="s">
         <v>70</v>
@@ -6883,13 +6862,13 @@
         <v>70</v>
       </c>
       <c r="N15" s="25" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="O15" s="25" t="s">
         <v>70</v>
       </c>
       <c r="P15" s="25" t="s">
-        <v>685</v>
+        <v>677</v>
       </c>
       <c r="Q15" s="25"/>
       <c r="R15" s="26"/>
@@ -6915,16 +6894,16 @@
         <v>68</v>
       </c>
       <c r="F16" s="33" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="G16" s="33" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="H16" s="34" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="I16" s="34" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="J16" s="25" t="s">
         <v>70</v>
@@ -6937,13 +6916,13 @@
         <v>70</v>
       </c>
       <c r="N16" s="25" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="O16" s="25" t="s">
         <v>70</v>
       </c>
       <c r="P16" s="25" t="s">
-        <v>685</v>
+        <v>677</v>
       </c>
       <c r="Q16" s="25"/>
       <c r="R16" s="26"/>
@@ -6983,13 +6962,13 @@
         <v>70</v>
       </c>
       <c r="N17" s="25" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="O17" s="25" t="s">
         <v>70</v>
       </c>
       <c r="P17" s="25" t="s">
-        <v>686</v>
+        <v>678</v>
       </c>
       <c r="Q17" s="25"/>
       <c r="R17" s="26" t="s">
@@ -7017,16 +6996,16 @@
         <v>73</v>
       </c>
       <c r="F18" s="33" t="s">
+        <v>538</v>
+      </c>
+      <c r="G18" s="33" t="s">
+        <v>538</v>
+      </c>
+      <c r="H18" s="34" t="s">
+        <v>539</v>
+      </c>
+      <c r="I18" s="34" t="s">
         <v>540</v>
-      </c>
-      <c r="G18" s="33" t="s">
-        <v>540</v>
-      </c>
-      <c r="H18" s="34" t="s">
-        <v>541</v>
-      </c>
-      <c r="I18" s="34" t="s">
-        <v>542</v>
       </c>
       <c r="J18" s="35" t="s">
         <v>517</v>
@@ -7041,11 +7020,11 @@
       <c r="N18" s="34" t="s">
         <v>518</v>
       </c>
-      <c r="O18" s="35" t="s">
-        <v>515</v>
-      </c>
-      <c r="P18" s="35" t="s">
-        <v>519</v>
+      <c r="O18" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="P18" s="25" t="s">
+        <v>679</v>
       </c>
       <c r="Q18" s="25"/>
       <c r="R18" s="26"/>
@@ -7071,16 +7050,16 @@
         <v>75</v>
       </c>
       <c r="F19" s="33" t="s">
+        <v>541</v>
+      </c>
+      <c r="G19" s="33" t="s">
+        <v>541</v>
+      </c>
+      <c r="H19" s="34" t="s">
+        <v>542</v>
+      </c>
+      <c r="I19" s="34" t="s">
         <v>543</v>
-      </c>
-      <c r="G19" s="33" t="s">
-        <v>543</v>
-      </c>
-      <c r="H19" s="34" t="s">
-        <v>544</v>
-      </c>
-      <c r="I19" s="34" t="s">
-        <v>545</v>
       </c>
       <c r="J19" s="35" t="s">
         <v>517</v>
@@ -7093,13 +7072,13 @@
         <v>70</v>
       </c>
       <c r="N19" s="35" t="s">
-        <v>520</v>
-      </c>
-      <c r="O19" s="35" t="s">
-        <v>515</v>
-      </c>
-      <c r="P19" s="35" t="s">
         <v>519</v>
+      </c>
+      <c r="O19" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="P19" s="25" t="s">
+        <v>679</v>
       </c>
       <c r="Q19" s="25"/>
       <c r="R19" s="26"/>
@@ -7125,16 +7104,16 @@
         <v>77</v>
       </c>
       <c r="F20" s="33" t="s">
+        <v>544</v>
+      </c>
+      <c r="G20" s="33" t="s">
+        <v>544</v>
+      </c>
+      <c r="H20" s="34" t="s">
+        <v>545</v>
+      </c>
+      <c r="I20" s="34" t="s">
         <v>546</v>
-      </c>
-      <c r="G20" s="33" t="s">
-        <v>546</v>
-      </c>
-      <c r="H20" s="34" t="s">
-        <v>547</v>
-      </c>
-      <c r="I20" s="34" t="s">
-        <v>548</v>
       </c>
       <c r="J20" s="35" t="s">
         <v>70</v>
@@ -7147,13 +7126,13 @@
         <v>70</v>
       </c>
       <c r="N20" s="35" t="s">
-        <v>520</v>
-      </c>
-      <c r="O20" s="35" t="s">
-        <v>515</v>
-      </c>
-      <c r="P20" s="35" t="s">
         <v>519</v>
+      </c>
+      <c r="O20" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="P20" s="25" t="s">
+        <v>679</v>
       </c>
       <c r="Q20" s="25"/>
       <c r="R20" s="26"/>
@@ -7179,16 +7158,16 @@
         <v>79</v>
       </c>
       <c r="F21" s="33" t="s">
+        <v>547</v>
+      </c>
+      <c r="G21" s="33" t="s">
+        <v>547</v>
+      </c>
+      <c r="H21" s="34" t="s">
+        <v>548</v>
+      </c>
+      <c r="I21" s="34" t="s">
         <v>549</v>
-      </c>
-      <c r="G21" s="33" t="s">
-        <v>549</v>
-      </c>
-      <c r="H21" s="34" t="s">
-        <v>550</v>
-      </c>
-      <c r="I21" s="34" t="s">
-        <v>551</v>
       </c>
       <c r="J21" s="35" t="s">
         <v>70</v>
@@ -7201,13 +7180,13 @@
         <v>70</v>
       </c>
       <c r="N21" s="35" t="s">
-        <v>520</v>
-      </c>
-      <c r="O21" s="35" t="s">
-        <v>515</v>
-      </c>
-      <c r="P21" s="35" t="s">
-        <v>522</v>
+        <v>519</v>
+      </c>
+      <c r="O21" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="P21" s="25" t="s">
+        <v>679</v>
       </c>
       <c r="Q21" s="25"/>
       <c r="R21" s="26"/>
@@ -7233,16 +7212,16 @@
         <v>81</v>
       </c>
       <c r="F22" s="33" t="s">
+        <v>550</v>
+      </c>
+      <c r="G22" s="33" t="s">
+        <v>550</v>
+      </c>
+      <c r="H22" s="34" t="s">
+        <v>551</v>
+      </c>
+      <c r="I22" s="34" t="s">
         <v>552</v>
-      </c>
-      <c r="G22" s="33" t="s">
-        <v>552</v>
-      </c>
-      <c r="H22" s="34" t="s">
-        <v>553</v>
-      </c>
-      <c r="I22" s="34" t="s">
-        <v>554</v>
       </c>
       <c r="J22" s="35" t="s">
         <v>70</v>
@@ -7255,13 +7234,13 @@
         <v>70</v>
       </c>
       <c r="N22" s="35" t="s">
-        <v>520</v>
-      </c>
-      <c r="O22" s="35" t="s">
-        <v>515</v>
-      </c>
-      <c r="P22" s="35" t="s">
-        <v>522</v>
+        <v>519</v>
+      </c>
+      <c r="O22" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="P22" s="25" t="s">
+        <v>679</v>
       </c>
       <c r="Q22" s="25"/>
       <c r="R22" s="26"/>
@@ -7287,16 +7266,16 @@
         <v>83</v>
       </c>
       <c r="F23" s="33" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="G23" s="33" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="H23" s="34" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="I23" s="34" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="J23" s="35" t="s">
         <v>70</v>
@@ -7309,13 +7288,13 @@
         <v>70</v>
       </c>
       <c r="N23" s="35" t="s">
-        <v>520</v>
-      </c>
-      <c r="O23" s="35" t="s">
-        <v>515</v>
-      </c>
-      <c r="P23" s="35" t="s">
-        <v>522</v>
+        <v>519</v>
+      </c>
+      <c r="O23" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="P23" s="25" t="s">
+        <v>679</v>
       </c>
       <c r="Q23" s="25"/>
       <c r="R23" s="26"/>
@@ -7348,7 +7327,7 @@
         <v>515</v>
       </c>
       <c r="K24" s="25" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="L24" s="25"/>
       <c r="M24" s="25"/>
@@ -7386,7 +7365,7 @@
         <v>515</v>
       </c>
       <c r="K25" s="25" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="L25" s="25"/>
       <c r="M25" s="25"/>
@@ -7417,16 +7396,16 @@
         <v>89</v>
       </c>
       <c r="F26" s="33" t="s">
+        <v>555</v>
+      </c>
+      <c r="G26" s="33" t="s">
+        <v>555</v>
+      </c>
+      <c r="H26" s="34" t="s">
+        <v>556</v>
+      </c>
+      <c r="I26" s="34" t="s">
         <v>557</v>
-      </c>
-      <c r="G26" s="33" t="s">
-        <v>557</v>
-      </c>
-      <c r="H26" s="34" t="s">
-        <v>558</v>
-      </c>
-      <c r="I26" s="34" t="s">
-        <v>559</v>
       </c>
       <c r="J26" s="35" t="s">
         <v>70</v>
@@ -7441,11 +7420,11 @@
       <c r="N26" s="34" t="s">
         <v>518</v>
       </c>
-      <c r="O26" s="35" t="s">
-        <v>515</v>
-      </c>
-      <c r="P26" s="35" t="s">
-        <v>519</v>
+      <c r="O26" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="P26" s="25" t="s">
+        <v>679</v>
       </c>
       <c r="Q26" s="25"/>
       <c r="R26" s="26"/>
@@ -7471,16 +7450,16 @@
         <v>91</v>
       </c>
       <c r="F27" s="33" t="s">
+        <v>558</v>
+      </c>
+      <c r="G27" s="33" t="s">
+        <v>558</v>
+      </c>
+      <c r="H27" s="34" t="s">
+        <v>559</v>
+      </c>
+      <c r="I27" s="34" t="s">
         <v>560</v>
-      </c>
-      <c r="G27" s="33" t="s">
-        <v>560</v>
-      </c>
-      <c r="H27" s="34" t="s">
-        <v>561</v>
-      </c>
-      <c r="I27" s="34" t="s">
-        <v>562</v>
       </c>
       <c r="J27" s="35" t="s">
         <v>70</v>
@@ -7495,11 +7474,11 @@
       <c r="N27" s="34" t="s">
         <v>518</v>
       </c>
-      <c r="O27" s="35" t="s">
-        <v>515</v>
-      </c>
-      <c r="P27" s="35" t="s">
-        <v>519</v>
+      <c r="O27" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="P27" s="25" t="s">
+        <v>679</v>
       </c>
       <c r="Q27" s="25"/>
       <c r="R27" s="26"/>
@@ -7525,16 +7504,16 @@
         <v>93</v>
       </c>
       <c r="F28" s="33" t="s">
+        <v>561</v>
+      </c>
+      <c r="G28" s="33" t="s">
+        <v>561</v>
+      </c>
+      <c r="H28" s="34" t="s">
+        <v>562</v>
+      </c>
+      <c r="I28" s="34" t="s">
         <v>563</v>
-      </c>
-      <c r="G28" s="33" t="s">
-        <v>563</v>
-      </c>
-      <c r="H28" s="34" t="s">
-        <v>564</v>
-      </c>
-      <c r="I28" s="34" t="s">
-        <v>565</v>
       </c>
       <c r="J28" s="35" t="s">
         <v>70</v>
@@ -7549,11 +7528,11 @@
       <c r="N28" s="34" t="s">
         <v>518</v>
       </c>
-      <c r="O28" s="35" t="s">
-        <v>515</v>
-      </c>
-      <c r="P28" s="35" t="s">
-        <v>519</v>
+      <c r="O28" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="P28" s="25" t="s">
+        <v>679</v>
       </c>
       <c r="Q28" s="25"/>
       <c r="R28" s="26"/>
@@ -7586,7 +7565,7 @@
         <v>515</v>
       </c>
       <c r="K29" s="25" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="L29" s="25"/>
       <c r="M29" s="25"/>
@@ -7624,7 +7603,7 @@
         <v>515</v>
       </c>
       <c r="K30" s="25" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="L30" s="25"/>
       <c r="M30" s="25"/>
@@ -7659,10 +7638,10 @@
       <c r="H31" s="24"/>
       <c r="I31" s="24"/>
       <c r="J31" s="25" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="K31" s="25" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="L31" s="25"/>
       <c r="M31" s="25"/>
@@ -7700,7 +7679,7 @@
         <v>515</v>
       </c>
       <c r="K32" s="25" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="L32" s="25"/>
       <c r="M32" s="25"/>
@@ -7735,10 +7714,10 @@
       <c r="H33" s="24"/>
       <c r="I33" s="24"/>
       <c r="J33" s="25" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="K33" s="25" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="L33" s="25"/>
       <c r="M33" s="25"/>
@@ -7773,10 +7752,10 @@
       <c r="H34" s="24"/>
       <c r="I34" s="24"/>
       <c r="J34" s="25" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="K34" s="25" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="L34" s="25"/>
       <c r="M34" s="25"/>
@@ -7814,7 +7793,7 @@
         <v>515</v>
       </c>
       <c r="K35" s="25" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="L35" s="25"/>
       <c r="M35" s="25"/>
@@ -7852,7 +7831,7 @@
         <v>515</v>
       </c>
       <c r="K36" s="25" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="L36" s="25"/>
       <c r="M36" s="25"/>
@@ -13867,16 +13846,16 @@
         <v>461</v>
       </c>
       <c r="F213" s="33" t="s">
+        <v>564</v>
+      </c>
+      <c r="G213" s="33" t="s">
+        <v>564</v>
+      </c>
+      <c r="H213" s="34" t="s">
+        <v>565</v>
+      </c>
+      <c r="I213" s="34" t="s">
         <v>566</v>
-      </c>
-      <c r="G213" s="33" t="s">
-        <v>566</v>
-      </c>
-      <c r="H213" s="34" t="s">
-        <v>567</v>
-      </c>
-      <c r="I213" s="34" t="s">
-        <v>568</v>
       </c>
       <c r="J213" s="25" t="s">
         <v>70</v>
@@ -13905,22 +13884,22 @@
         <v>66</v>
       </c>
       <c r="D214" s="39" t="s">
+        <v>567</v>
+      </c>
+      <c r="E214" s="40" t="s">
+        <v>568</v>
+      </c>
+      <c r="F214" s="33" t="s">
         <v>569</v>
       </c>
-      <c r="E214" s="40" t="s">
+      <c r="G214" s="33" t="s">
+        <v>569</v>
+      </c>
+      <c r="H214" s="34" t="s">
         <v>570</v>
       </c>
-      <c r="F214" s="33" t="s">
-        <v>571</v>
-      </c>
-      <c r="G214" s="33" t="s">
-        <v>571</v>
-      </c>
-      <c r="H214" s="34" t="s">
-        <v>572</v>
-      </c>
       <c r="I214" s="34" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="J214" s="25" t="s">
         <v>70</v>
@@ -13933,13 +13912,13 @@
         <v>70</v>
       </c>
       <c r="N214" s="25" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="O214" s="25" t="s">
         <v>70</v>
       </c>
       <c r="P214" s="25" t="s">
-        <v>574</v>
+        <v>677</v>
       </c>
       <c r="Q214" s="41"/>
       <c r="R214" s="42"/>
@@ -13959,22 +13938,22 @@
         <v>66</v>
       </c>
       <c r="D215" s="39" t="s">
+        <v>572</v>
+      </c>
+      <c r="E215" s="40" t="s">
+        <v>573</v>
+      </c>
+      <c r="F215" s="33" t="s">
+        <v>574</v>
+      </c>
+      <c r="G215" s="33" t="s">
+        <v>574</v>
+      </c>
+      <c r="H215" s="34" t="s">
         <v>575</v>
       </c>
-      <c r="E215" s="40" t="s">
-        <v>576</v>
-      </c>
-      <c r="F215" s="33" t="s">
-        <v>577</v>
-      </c>
-      <c r="G215" s="33" t="s">
-        <v>577</v>
-      </c>
-      <c r="H215" s="34" t="s">
-        <v>578</v>
-      </c>
       <c r="I215" s="34" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="J215" s="25" t="s">
         <v>70</v>
@@ -13987,13 +13966,13 @@
         <v>70</v>
       </c>
       <c r="N215" s="25" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="O215" s="25" t="s">
         <v>70</v>
       </c>
       <c r="P215" s="25" t="s">
-        <v>574</v>
+        <v>677</v>
       </c>
       <c r="Q215" s="41"/>
       <c r="R215" s="42"/>
@@ -14013,7 +13992,7 @@
         <v>66</v>
       </c>
       <c r="D216" s="39" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="E216" s="40" t="s">
         <v>69</v>
@@ -14033,13 +14012,13 @@
         <v>70</v>
       </c>
       <c r="N216" s="25" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="O216" s="25" t="s">
         <v>70</v>
       </c>
       <c r="P216" s="25" t="s">
-        <v>581</v>
+        <v>678</v>
       </c>
       <c r="Q216" s="41"/>
       <c r="R216" s="42" t="s">
@@ -14061,22 +14040,22 @@
         <v>66</v>
       </c>
       <c r="D217" s="39" t="s">
+        <v>578</v>
+      </c>
+      <c r="E217" s="40" t="s">
+        <v>579</v>
+      </c>
+      <c r="F217" s="33" t="s">
+        <v>580</v>
+      </c>
+      <c r="G217" s="33" t="s">
+        <v>580</v>
+      </c>
+      <c r="H217" s="34" t="s">
+        <v>581</v>
+      </c>
+      <c r="I217" s="34" t="s">
         <v>582</v>
-      </c>
-      <c r="E217" s="40" t="s">
-        <v>583</v>
-      </c>
-      <c r="F217" s="33" t="s">
-        <v>584</v>
-      </c>
-      <c r="G217" s="33" t="s">
-        <v>584</v>
-      </c>
-      <c r="H217" s="34" t="s">
-        <v>585</v>
-      </c>
-      <c r="I217" s="34" t="s">
-        <v>586</v>
       </c>
       <c r="J217" s="25" t="s">
         <v>70</v>
@@ -14105,10 +14084,10 @@
         <v>66</v>
       </c>
       <c r="D218" s="39" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="E218" s="40" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="F218" s="46"/>
       <c r="G218" s="45"/>
@@ -14118,7 +14097,7 @@
         <v>515</v>
       </c>
       <c r="K218" s="37" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="L218" s="41"/>
       <c r="M218" s="41"/>
@@ -14143,10 +14122,10 @@
         <v>66</v>
       </c>
       <c r="D219" s="39" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="E219" s="40" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="F219" s="46"/>
       <c r="G219" s="45"/>
@@ -14156,7 +14135,7 @@
         <v>515</v>
       </c>
       <c r="K219" s="37" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="L219" s="41"/>
       <c r="M219" s="41"/>
@@ -14181,10 +14160,10 @@
         <v>66</v>
       </c>
       <c r="D220" s="39" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="E220" s="40" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="F220" s="46"/>
       <c r="G220" s="45"/>
@@ -14194,7 +14173,7 @@
         <v>515</v>
       </c>
       <c r="K220" s="37" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="L220" s="41"/>
       <c r="M220" s="41"/>
@@ -14219,22 +14198,22 @@
         <v>66</v>
       </c>
       <c r="D221" s="39" t="s">
+        <v>589</v>
+      </c>
+      <c r="E221" s="22" t="s">
+        <v>590</v>
+      </c>
+      <c r="F221" s="33" t="s">
+        <v>591</v>
+      </c>
+      <c r="G221" s="33" t="s">
+        <v>591</v>
+      </c>
+      <c r="H221" s="34" t="s">
+        <v>592</v>
+      </c>
+      <c r="I221" s="34" t="s">
         <v>593</v>
-      </c>
-      <c r="E221" s="22" t="s">
-        <v>594</v>
-      </c>
-      <c r="F221" s="33" t="s">
-        <v>595</v>
-      </c>
-      <c r="G221" s="33" t="s">
-        <v>595</v>
-      </c>
-      <c r="H221" s="34" t="s">
-        <v>596</v>
-      </c>
-      <c r="I221" s="34" t="s">
-        <v>597</v>
       </c>
       <c r="J221" s="25" t="s">
         <v>70</v>
@@ -14250,10 +14229,10 @@
         <v>518</v>
       </c>
       <c r="O221" s="25" t="s">
-        <v>515</v>
+        <v>70</v>
       </c>
       <c r="P221" s="25" t="s">
-        <v>519</v>
+        <v>679</v>
       </c>
       <c r="Q221" s="41"/>
       <c r="R221" s="42"/>
@@ -14273,22 +14252,22 @@
         <v>66</v>
       </c>
       <c r="D222" s="39" t="s">
+        <v>594</v>
+      </c>
+      <c r="E222" s="40" t="s">
+        <v>595</v>
+      </c>
+      <c r="F222" s="33" t="s">
+        <v>596</v>
+      </c>
+      <c r="G222" s="33" t="s">
+        <v>596</v>
+      </c>
+      <c r="H222" s="34" t="s">
+        <v>597</v>
+      </c>
+      <c r="I222" s="34" t="s">
         <v>598</v>
-      </c>
-      <c r="E222" s="40" t="s">
-        <v>599</v>
-      </c>
-      <c r="F222" s="33" t="s">
-        <v>600</v>
-      </c>
-      <c r="G222" s="33" t="s">
-        <v>600</v>
-      </c>
-      <c r="H222" s="34" t="s">
-        <v>601</v>
-      </c>
-      <c r="I222" s="34" t="s">
-        <v>602</v>
       </c>
       <c r="J222" s="25" t="s">
         <v>70</v>
@@ -14301,13 +14280,13 @@
         <v>70</v>
       </c>
       <c r="N222" s="25" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="O222" s="25" t="s">
-        <v>515</v>
+        <v>70</v>
       </c>
       <c r="P222" s="25" t="s">
-        <v>603</v>
+        <v>679</v>
       </c>
       <c r="Q222" s="41"/>
       <c r="R222" s="42"/>
@@ -14327,22 +14306,22 @@
         <v>66</v>
       </c>
       <c r="D223" s="39" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="E223" s="40" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="F223" s="33" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
       <c r="G223" s="33" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
       <c r="H223" s="34" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
       <c r="I223" s="34" t="s">
-        <v>608</v>
+        <v>603</v>
       </c>
       <c r="J223" s="25" t="s">
         <v>70</v>
@@ -14358,10 +14337,10 @@
         <v>518</v>
       </c>
       <c r="O223" s="25" t="s">
-        <v>515</v>
+        <v>70</v>
       </c>
       <c r="P223" s="25" t="s">
-        <v>519</v>
+        <v>679</v>
       </c>
       <c r="Q223" s="41"/>
       <c r="R223" s="42"/>
@@ -14381,22 +14360,22 @@
         <v>66</v>
       </c>
       <c r="D224" s="39" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
       <c r="E224" s="40" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="F224" s="33" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
       <c r="G224" s="33" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
       <c r="H224" s="34" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
       <c r="I224" s="34" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
       <c r="J224" s="25" t="s">
         <v>70</v>
@@ -14412,10 +14391,10 @@
         <v>518</v>
       </c>
       <c r="O224" s="25" t="s">
-        <v>515</v>
+        <v>70</v>
       </c>
       <c r="P224" s="25" t="s">
-        <v>519</v>
+        <v>679</v>
       </c>
       <c r="Q224" s="41"/>
       <c r="R224" s="42"/>
@@ -14435,22 +14414,22 @@
         <v>66</v>
       </c>
       <c r="D225" s="39" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="E225" s="40" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="F225" s="33" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
       <c r="G225" s="33" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
       <c r="H225" s="34" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
       <c r="I225" s="34" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="J225" s="25" t="s">
         <v>70</v>
@@ -14466,10 +14445,10 @@
         <v>518</v>
       </c>
       <c r="O225" s="25" t="s">
-        <v>515</v>
+        <v>70</v>
       </c>
       <c r="P225" s="25" t="s">
-        <v>519</v>
+        <v>679</v>
       </c>
       <c r="Q225" s="41"/>
       <c r="R225" s="42"/>
@@ -14489,22 +14468,22 @@
         <v>66</v>
       </c>
       <c r="D226" s="39" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="E226" s="40" t="s">
-        <v>620</v>
+        <v>615</v>
       </c>
       <c r="F226" s="33" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="G226" s="33" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="H226" s="34" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="I226" s="34" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
       <c r="J226" s="25" t="s">
         <v>70</v>
@@ -14517,13 +14496,13 @@
         <v>70</v>
       </c>
       <c r="N226" s="25" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="O226" s="25" t="s">
-        <v>515</v>
+        <v>70</v>
       </c>
       <c r="P226" s="25" t="s">
-        <v>519</v>
+        <v>679</v>
       </c>
       <c r="Q226" s="41"/>
       <c r="R226" s="42"/>
@@ -14543,10 +14522,10 @@
         <v>66</v>
       </c>
       <c r="D227" s="39" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="E227" s="40" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
       <c r="F227" s="46"/>
       <c r="G227" s="45"/>
@@ -14556,7 +14535,7 @@
         <v>515</v>
       </c>
       <c r="K227" s="25" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
       <c r="L227" s="41"/>
       <c r="M227" s="41"/>
@@ -14581,22 +14560,22 @@
         <v>66</v>
       </c>
       <c r="D228" s="39" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="E228" s="40" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="F228" s="33" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
       <c r="G228" s="33" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
       <c r="H228" s="34" t="s">
-        <v>631</v>
+        <v>626</v>
       </c>
       <c r="I228" s="34" t="s">
-        <v>632</v>
+        <v>627</v>
       </c>
       <c r="J228" s="25" t="s">
         <v>70</v>
@@ -14609,13 +14588,13 @@
         <v>70</v>
       </c>
       <c r="N228" s="25" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="O228" s="25" t="s">
-        <v>515</v>
+        <v>70</v>
       </c>
       <c r="P228" s="25" t="s">
-        <v>633</v>
+        <v>679</v>
       </c>
       <c r="Q228" s="41"/>
       <c r="R228" s="42"/>
@@ -14635,22 +14614,22 @@
         <v>66</v>
       </c>
       <c r="D229" s="39" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="E229" s="40" t="s">
-        <v>635</v>
+        <v>629</v>
       </c>
       <c r="F229" s="33" t="s">
-        <v>636</v>
+        <v>630</v>
       </c>
       <c r="G229" s="33" t="s">
-        <v>636</v>
+        <v>630</v>
       </c>
       <c r="H229" s="34" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
       <c r="I229" s="34" t="s">
-        <v>638</v>
+        <v>632</v>
       </c>
       <c r="J229" s="25" t="s">
         <v>70</v>
@@ -14666,10 +14645,10 @@
         <v>518</v>
       </c>
       <c r="O229" s="25" t="s">
-        <v>515</v>
+        <v>70</v>
       </c>
       <c r="P229" s="25" t="s">
-        <v>633</v>
+        <v>679</v>
       </c>
       <c r="Q229" s="41"/>
       <c r="R229" s="42"/>
@@ -14689,22 +14668,22 @@
         <v>66</v>
       </c>
       <c r="D230" s="39" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
       <c r="E230" s="40" t="s">
-        <v>640</v>
+        <v>634</v>
       </c>
       <c r="F230" s="33" t="s">
-        <v>641</v>
+        <v>635</v>
       </c>
       <c r="G230" s="33" t="s">
-        <v>641</v>
+        <v>635</v>
       </c>
       <c r="H230" s="34" t="s">
-        <v>642</v>
+        <v>636</v>
       </c>
       <c r="I230" s="34" t="s">
-        <v>643</v>
+        <v>637</v>
       </c>
       <c r="J230" s="25" t="s">
         <v>70</v>
@@ -14720,10 +14699,10 @@
         <v>518</v>
       </c>
       <c r="O230" s="25" t="s">
-        <v>515</v>
+        <v>70</v>
       </c>
       <c r="P230" s="25" t="s">
-        <v>644</v>
+        <v>679</v>
       </c>
       <c r="Q230" s="41"/>
       <c r="R230" s="42"/>
@@ -14743,22 +14722,22 @@
         <v>66</v>
       </c>
       <c r="D231" s="39" t="s">
-        <v>645</v>
+        <v>638</v>
       </c>
       <c r="E231" s="40" t="s">
-        <v>646</v>
+        <v>639</v>
       </c>
       <c r="F231" s="33" t="s">
-        <v>647</v>
+        <v>640</v>
       </c>
       <c r="G231" s="33" t="s">
-        <v>647</v>
+        <v>640</v>
       </c>
       <c r="H231" s="34" t="s">
-        <v>648</v>
+        <v>641</v>
       </c>
       <c r="I231" s="34" t="s">
-        <v>649</v>
+        <v>642</v>
       </c>
       <c r="J231" s="25" t="s">
         <v>70</v>
@@ -14771,13 +14750,13 @@
         <v>70</v>
       </c>
       <c r="N231" s="25" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="O231" s="25" t="s">
-        <v>515</v>
+        <v>70</v>
       </c>
       <c r="P231" s="25" t="s">
-        <v>650</v>
+        <v>679</v>
       </c>
       <c r="Q231" s="41"/>
       <c r="R231" s="42"/>
@@ -14797,10 +14776,10 @@
         <v>66</v>
       </c>
       <c r="D232" s="39" t="s">
-        <v>651</v>
+        <v>643</v>
       </c>
       <c r="E232" s="40" t="s">
-        <v>652</v>
+        <v>644</v>
       </c>
       <c r="F232" s="46"/>
       <c r="G232" s="45"/>
@@ -14810,7 +14789,7 @@
         <v>515</v>
       </c>
       <c r="K232" s="25" t="s">
-        <v>653</v>
+        <v>645</v>
       </c>
       <c r="L232" s="41"/>
       <c r="M232" s="41"/>
@@ -14835,22 +14814,22 @@
         <v>66</v>
       </c>
       <c r="D233" s="39" t="s">
-        <v>654</v>
+        <v>646</v>
       </c>
       <c r="E233" s="40" t="s">
-        <v>655</v>
+        <v>647</v>
       </c>
       <c r="F233" s="33" t="s">
-        <v>656</v>
+        <v>648</v>
       </c>
       <c r="G233" s="33" t="s">
-        <v>656</v>
+        <v>648</v>
       </c>
       <c r="H233" s="34" t="s">
-        <v>657</v>
+        <v>649</v>
       </c>
       <c r="I233" s="34" t="s">
-        <v>658</v>
+        <v>650</v>
       </c>
       <c r="J233" s="25" t="s">
         <v>70</v>
@@ -14863,13 +14842,13 @@
         <v>70</v>
       </c>
       <c r="N233" s="41" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="O233" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="P233" s="41" t="s">
-        <v>687</v>
+      <c r="P233" s="25" t="s">
+        <v>679</v>
       </c>
       <c r="Q233" s="41"/>
       <c r="R233" s="42"/>
@@ -14889,10 +14868,10 @@
         <v>66</v>
       </c>
       <c r="D234" s="39" t="s">
-        <v>659</v>
+        <v>651</v>
       </c>
       <c r="E234" s="40" t="s">
-        <v>660</v>
+        <v>652</v>
       </c>
       <c r="F234" s="46"/>
       <c r="G234" s="45"/>
@@ -14902,7 +14881,7 @@
         <v>515</v>
       </c>
       <c r="K234" s="25" t="s">
-        <v>661</v>
+        <v>653</v>
       </c>
       <c r="L234" s="41"/>
       <c r="M234" s="41"/>
@@ -14927,10 +14906,10 @@
         <v>66</v>
       </c>
       <c r="D235" s="39" t="s">
-        <v>662</v>
+        <v>654</v>
       </c>
       <c r="E235" s="40" t="s">
-        <v>663</v>
+        <v>655</v>
       </c>
       <c r="F235" s="46"/>
       <c r="G235" s="45"/>
@@ -14940,7 +14919,7 @@
         <v>515</v>
       </c>
       <c r="K235" s="25" t="s">
-        <v>664</v>
+        <v>656</v>
       </c>
       <c r="L235" s="41"/>
       <c r="M235" s="41"/>
@@ -14965,10 +14944,10 @@
         <v>66</v>
       </c>
       <c r="D236" s="39" t="s">
-        <v>665</v>
+        <v>657</v>
       </c>
       <c r="E236" s="40" t="s">
-        <v>666</v>
+        <v>658</v>
       </c>
       <c r="F236" s="46"/>
       <c r="G236" s="45"/>
@@ -14978,7 +14957,7 @@
         <v>515</v>
       </c>
       <c r="K236" s="25" t="s">
-        <v>664</v>
+        <v>656</v>
       </c>
       <c r="L236" s="41"/>
       <c r="M236" s="41"/>
@@ -15003,10 +14982,10 @@
         <v>66</v>
       </c>
       <c r="D237" s="39" t="s">
-        <v>667</v>
+        <v>659</v>
       </c>
       <c r="E237" s="40" t="s">
-        <v>668</v>
+        <v>660</v>
       </c>
       <c r="F237" s="46"/>
       <c r="G237" s="45"/>
@@ -15016,7 +14995,7 @@
         <v>515</v>
       </c>
       <c r="K237" s="25" t="s">
-        <v>661</v>
+        <v>653</v>
       </c>
       <c r="L237" s="41"/>
       <c r="M237" s="41"/>
@@ -15041,10 +15020,10 @@
         <v>66</v>
       </c>
       <c r="D238" s="39" t="s">
-        <v>669</v>
+        <v>661</v>
       </c>
       <c r="E238" s="40" t="s">
-        <v>670</v>
+        <v>662</v>
       </c>
       <c r="F238" s="46"/>
       <c r="G238" s="45"/>
@@ -15054,7 +15033,7 @@
         <v>515</v>
       </c>
       <c r="K238" s="25" t="s">
-        <v>661</v>
+        <v>653</v>
       </c>
       <c r="L238" s="41"/>
       <c r="M238" s="41"/>
@@ -15079,22 +15058,22 @@
         <v>66</v>
       </c>
       <c r="D239" s="39" t="s">
-        <v>671</v>
+        <v>663</v>
       </c>
       <c r="E239" s="40" t="s">
-        <v>672</v>
+        <v>664</v>
       </c>
       <c r="F239" s="33" t="s">
-        <v>673</v>
+        <v>665</v>
       </c>
       <c r="G239" s="33" t="s">
-        <v>673</v>
+        <v>665</v>
       </c>
       <c r="H239" s="34" t="s">
-        <v>674</v>
+        <v>666</v>
       </c>
       <c r="I239" s="34" t="s">
-        <v>675</v>
+        <v>667</v>
       </c>
       <c r="J239" s="25" t="s">
         <v>70</v>
@@ -15107,13 +15086,13 @@
         <v>70</v>
       </c>
       <c r="N239" s="25" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="O239" s="25" t="s">
-        <v>515</v>
+        <v>70</v>
       </c>
       <c r="P239" s="25" t="s">
-        <v>650</v>
+        <v>679</v>
       </c>
       <c r="Q239" s="41"/>
       <c r="R239" s="42"/>
@@ -15133,22 +15112,22 @@
         <v>66</v>
       </c>
       <c r="D240" s="39" t="s">
-        <v>676</v>
+        <v>668</v>
       </c>
       <c r="E240" s="40" t="s">
-        <v>677</v>
+        <v>669</v>
       </c>
       <c r="F240" s="33" t="s">
-        <v>678</v>
+        <v>670</v>
       </c>
       <c r="G240" s="33" t="s">
-        <v>678</v>
+        <v>670</v>
       </c>
       <c r="H240" s="34" t="s">
-        <v>679</v>
+        <v>671</v>
       </c>
       <c r="I240" s="34" t="s">
-        <v>680</v>
+        <v>672</v>
       </c>
       <c r="J240" s="41" t="s">
         <v>70</v>
@@ -19359,7 +19338,7 @@
       <c r="T830" s="13"/>
     </row>
   </sheetData>
-  <autoFilter ref="A9:T213" xr:uid="{00000000-0009-0000-0000-000002000000}">
+  <autoFilter ref="A9:T240" xr:uid="{00000000-0009-0000-0000-000002000000}">
     <filterColumn colId="1">
       <filters>
         <filter val="VALIDAZIONE"/>

</xml_diff>